<commit_message>
DOCS : for insertSupplyInDB
</commit_message>
<xml_diff>
--- a/supply(test).xlsx
+++ b/supply(test).xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="77">
   <si>
     <t>공급코드</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -38,50 +38,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>A190507001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A190507002</t>
-  </si>
-  <si>
-    <t>A190507003</t>
-  </si>
-  <si>
-    <t>A190507004</t>
-  </si>
-  <si>
-    <t>A190507005</t>
-  </si>
-  <si>
-    <t>A190507006</t>
-  </si>
-  <si>
-    <t>A190507007</t>
-  </si>
-  <si>
-    <t>A190507008</t>
-  </si>
-  <si>
-    <t>A190508001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A190508002</t>
-  </si>
-  <si>
-    <t>A190508003</t>
-  </si>
-  <si>
-    <t>A190508004</t>
-  </si>
-  <si>
-    <t>A190508005</t>
-  </si>
-  <si>
-    <t>A190508006</t>
-  </si>
-  <si>
     <t>A101</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -133,22 +89,6 @@
     <t>A106</t>
   </si>
   <si>
-    <t>A190505001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A190505002</t>
-  </si>
-  <si>
-    <t>A190505003</t>
-  </si>
-  <si>
-    <t>A190505004</t>
-  </si>
-  <si>
-    <t>A190505005</t>
-  </si>
-  <si>
     <t>A105</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -169,138 +109,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>A190707001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A190707002</t>
-  </si>
-  <si>
-    <t>A190707003</t>
-  </si>
-  <si>
-    <t>A190707004</t>
-  </si>
-  <si>
-    <t>A190707005</t>
-  </si>
-  <si>
-    <t>A190707006</t>
-  </si>
-  <si>
-    <t>A105</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A102</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A104</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A109</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A190705001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A190705002</t>
-  </si>
-  <si>
-    <t>A190705003</t>
-  </si>
-  <si>
-    <t>A190705004</t>
-  </si>
-  <si>
-    <t>B190507001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B190507002</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B190507003</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B190507004</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B190507005</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B190507006</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C190508001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C190508002</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C190508003</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C190508004</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C190508005</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C190508006</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D190505001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D190505002</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D190505003</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D190505004</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>D190505005</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E190705001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E190705002</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E190705003</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E190705004</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>B101</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -355,17 +163,118 @@
     <t>D109</t>
   </si>
   <si>
-    <t>E102</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>E103</t>
-  </si>
-  <si>
-    <t>E104</t>
-  </si>
-  <si>
-    <t>E105</t>
+    <t>A190505101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A190505102</t>
+  </si>
+  <si>
+    <t>A190505103</t>
+  </si>
+  <si>
+    <t>A190505104</t>
+  </si>
+  <si>
+    <t>A190505105</t>
+  </si>
+  <si>
+    <t>A190507101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A190507102</t>
+  </si>
+  <si>
+    <t>A190507103</t>
+  </si>
+  <si>
+    <t>A190507104</t>
+  </si>
+  <si>
+    <t>A190507105</t>
+  </si>
+  <si>
+    <t>A190507106</t>
+  </si>
+  <si>
+    <t>A190507107</t>
+  </si>
+  <si>
+    <t>A190507108</t>
+  </si>
+  <si>
+    <t>A190508101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A190508102</t>
+  </si>
+  <si>
+    <t>A190508103</t>
+  </si>
+  <si>
+    <t>A190508104</t>
+  </si>
+  <si>
+    <t>A190508105</t>
+  </si>
+  <si>
+    <t>A190508106</t>
+  </si>
+  <si>
+    <t>B190507101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B190507102</t>
+  </si>
+  <si>
+    <t>B190507103</t>
+  </si>
+  <si>
+    <t>B190507104</t>
+  </si>
+  <si>
+    <t>B190507105</t>
+  </si>
+  <si>
+    <t>B190507106</t>
+  </si>
+  <si>
+    <t>C190508101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C190508102</t>
+  </si>
+  <si>
+    <t>C190508103</t>
+  </si>
+  <si>
+    <t>C190508104</t>
+  </si>
+  <si>
+    <t>C190508105</t>
+  </si>
+  <si>
+    <t>C190508106</t>
+  </si>
+  <si>
+    <t>D190505101</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D190505102</t>
+  </si>
+  <si>
+    <t>D190505103</t>
+  </si>
+  <si>
+    <t>D190505104</t>
+  </si>
+  <si>
+    <t>D190505105</t>
   </si>
 </sst>
 </file>
@@ -753,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:XFD38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -787,10 +696,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2">
         <v>43590.3125</v>
@@ -804,10 +713,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="C3" s="2">
         <v>43590.3125</v>
@@ -821,10 +730,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="C4" s="2">
         <v>43590.3125</v>
@@ -838,10 +747,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>41</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2">
         <v>43590.3125</v>
@@ -855,10 +764,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C6" s="2">
         <v>43590.3125</v>
@@ -872,13 +781,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>72</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="C7" s="2">
-        <v>43592.416666666664</v>
+        <v>43590.3125</v>
       </c>
       <c r="D7" s="1">
         <v>100</v>
@@ -889,13 +798,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>73</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="C8" s="2">
-        <v>43592.416666666664</v>
+        <v>43590.3125</v>
       </c>
       <c r="D8" s="1">
         <v>100</v>
@@ -906,13 +815,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>74</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C9" s="2">
-        <v>43592.416666666664</v>
+        <v>43590.3125</v>
       </c>
       <c r="D9" s="1">
         <v>100</v>
@@ -923,13 +832,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="C10" s="2">
-        <v>43592.416666666664</v>
+        <v>43590.3125</v>
       </c>
       <c r="D10" s="1">
         <v>100</v>
@@ -940,13 +849,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="C11" s="2">
-        <v>43592.416666666664</v>
+        <v>43590.3125</v>
       </c>
       <c r="D11" s="1">
         <v>100</v>
@@ -957,10 +866,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C12" s="2">
         <v>43592.416666666664</v>
@@ -974,10 +883,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>47</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="C13" s="2">
         <v>43592.416666666664</v>
@@ -991,10 +900,10 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>48</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="C14" s="2">
         <v>43592.416666666664</v>
@@ -1008,13 +917,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>49</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="C15" s="2">
-        <v>43593.5</v>
+        <v>43592.416666666664</v>
       </c>
       <c r="D15" s="1">
         <v>100</v>
@@ -1025,13 +934,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C16" s="2">
-        <v>43593.5</v>
+        <v>43592.416666666664</v>
       </c>
       <c r="D16" s="1">
         <v>100</v>
@@ -1042,13 +951,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="C17" s="2">
-        <v>43593.5</v>
+        <v>43592.416666666664</v>
       </c>
       <c r="D17" s="1">
         <v>100</v>
@@ -1059,13 +968,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="C18" s="2">
-        <v>43593.5</v>
+        <v>43592.416666666664</v>
       </c>
       <c r="D18" s="1">
         <v>100</v>
@@ -1076,13 +985,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="C19" s="2">
-        <v>43593.5</v>
+        <v>43592.416666666664</v>
       </c>
       <c r="D19" s="1">
         <v>100</v>
@@ -1093,13 +1002,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="C20" s="2">
-        <v>43593.5</v>
+        <v>43592.416666666664</v>
       </c>
       <c r="D20" s="1">
         <v>100</v>
@@ -1110,13 +1019,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C21" s="2">
-        <v>43653.916666666664</v>
+        <v>43592.416666666664</v>
       </c>
       <c r="D21" s="1">
         <v>100</v>
@@ -1127,13 +1036,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C22" s="2">
-        <v>43653.916666666664</v>
+        <v>43592.416666666664</v>
       </c>
       <c r="D22" s="1">
         <v>100</v>
@@ -1144,13 +1053,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C23" s="2">
-        <v>43653.916666666664</v>
+        <v>43592.416666666664</v>
       </c>
       <c r="D23" s="1">
         <v>100</v>
@@ -1161,13 +1070,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C24" s="2">
-        <v>43653.916666666664</v>
+        <v>43592.416666666664</v>
       </c>
       <c r="D24" s="1">
         <v>100</v>
@@ -1178,13 +1087,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C25" s="2">
-        <v>43653.916666666664</v>
+        <v>43592.416666666664</v>
       </c>
       <c r="D25" s="1">
         <v>100</v>
@@ -1195,13 +1104,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="C26" s="2">
-        <v>43653.916666666664</v>
+        <v>43593.5</v>
       </c>
       <c r="D26" s="1">
         <v>100</v>
@@ -1212,13 +1121,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="C27" s="2">
-        <v>43651.333333333336</v>
+        <v>43593.5</v>
       </c>
       <c r="D27" s="1">
         <v>100</v>
@@ -1229,13 +1138,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>51</v>
+        <v>15</v>
       </c>
       <c r="C28" s="2">
-        <v>43651.333333333336</v>
+        <v>43593.5</v>
       </c>
       <c r="D28" s="1">
         <v>100</v>
@@ -1246,13 +1155,13 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="C29" s="2">
-        <v>43651.333333333336</v>
+        <v>43593.5</v>
       </c>
       <c r="D29" s="1">
         <v>100</v>
@@ -1263,13 +1172,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="C30" s="2">
-        <v>43651.333333333336</v>
+        <v>43593.5</v>
       </c>
       <c r="D30" s="1">
         <v>100</v>
@@ -1280,13 +1189,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>78</v>
+        <v>18</v>
       </c>
       <c r="C31" s="2">
-        <v>43592.416666666664</v>
+        <v>43593.5</v>
       </c>
       <c r="D31" s="1">
         <v>100</v>
@@ -1297,13 +1206,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>79</v>
+        <v>30</v>
       </c>
       <c r="C32" s="2">
-        <v>43592.416666666664</v>
+        <v>43593.5</v>
       </c>
       <c r="D32" s="1">
         <v>100</v>
@@ -1314,13 +1223,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>80</v>
+        <v>31</v>
       </c>
       <c r="C33" s="2">
-        <v>43592.416666666664</v>
+        <v>43593.5</v>
       </c>
       <c r="D33" s="1">
         <v>100</v>
@@ -1331,13 +1240,13 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>81</v>
+        <v>32</v>
       </c>
       <c r="C34" s="2">
-        <v>43592.416666666664</v>
+        <v>43593.5</v>
       </c>
       <c r="D34" s="1">
         <v>100</v>
@@ -1348,13 +1257,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>82</v>
+        <v>33</v>
       </c>
       <c r="C35" s="2">
-        <v>43592.416666666664</v>
+        <v>43593.5</v>
       </c>
       <c r="D35" s="1">
         <v>100</v>
@@ -1365,13 +1274,13 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>83</v>
+        <v>34</v>
       </c>
       <c r="C36" s="2">
-        <v>43592.416666666664</v>
+        <v>43593.5</v>
       </c>
       <c r="D36" s="1">
         <v>100</v>
@@ -1382,10 +1291,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
       <c r="C37" s="2">
         <v>43593.5</v>
@@ -1397,247 +1306,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C38" s="2">
-        <v>43593.5</v>
-      </c>
-      <c r="D38" s="1">
-        <v>100</v>
-      </c>
-      <c r="E38" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C39" s="2">
-        <v>43593.5</v>
-      </c>
-      <c r="D39" s="1">
-        <v>100</v>
-      </c>
-      <c r="E39" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C40" s="2">
-        <v>43593.5</v>
-      </c>
-      <c r="D40" s="1">
-        <v>100</v>
-      </c>
-      <c r="E40" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C41" s="2">
-        <v>43593.5</v>
-      </c>
-      <c r="D41" s="1">
-        <v>100</v>
-      </c>
-      <c r="E41" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C42" s="2">
-        <v>43593.5</v>
-      </c>
-      <c r="D42" s="1">
-        <v>100</v>
-      </c>
-      <c r="E42" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C43" s="2">
-        <v>43590.3125</v>
-      </c>
-      <c r="D43" s="1">
-        <v>100</v>
-      </c>
-      <c r="E43" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C44" s="2">
-        <v>43590.3125</v>
-      </c>
-      <c r="D44" s="1">
-        <v>100</v>
-      </c>
-      <c r="E44" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C45" s="2">
-        <v>43590.3125</v>
-      </c>
-      <c r="D45" s="1">
-        <v>100</v>
-      </c>
-      <c r="E45" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C46" s="2">
-        <v>43590.3125</v>
-      </c>
-      <c r="D46" s="1">
-        <v>100</v>
-      </c>
-      <c r="E46" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C47" s="2">
-        <v>43590.3125</v>
-      </c>
-      <c r="D47" s="1">
-        <v>100</v>
-      </c>
-      <c r="E47" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C48" s="2">
-        <v>43651.333333333336</v>
-      </c>
-      <c r="D48" s="1">
-        <v>100</v>
-      </c>
-      <c r="E48" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C49" s="2">
-        <v>43651.333333333336</v>
-      </c>
-      <c r="D49" s="1">
-        <v>100</v>
-      </c>
-      <c r="E49" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C50" s="2">
-        <v>43651.333333333336</v>
-      </c>
-      <c r="D50" s="1">
-        <v>100</v>
-      </c>
-      <c r="E50" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C51" s="2">
-        <v>43651.333333333336</v>
-      </c>
-      <c r="D51" s="1">
-        <v>100</v>
-      </c>
-      <c r="E51" s="1">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
-  <sortState ref="A2:E20">
-    <sortCondition ref="C2:C20"/>
+  <sortState ref="A2:E51">
+    <sortCondition ref="C2:C51"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>